<commit_message>
Changes with team additions
</commit_message>
<xml_diff>
--- a/April_2024/Complete/MLS.xlsx
+++ b/April_2024/Complete/MLS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://spgl-my.sharepoint.com/personal/kirt_raynes_spglobal_com/Documents/Documents/Notebooks/NBA Teams/April_2024/Complete/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_2B01AF46D864F00E62355476585DCE3A874713BE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{005D53E1-B0DA-498B-A0C4-D3905678FEA8}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_2B01AF46D864F00E62355476585DCE3A874713BE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C062E71-89D9-4337-B451-93E2EA20F6A6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -493,9 +493,6 @@
     <t>https://twitter.com/SoundersFC</t>
   </si>
   <si>
-    <t>https://www.youtube.com/channel/UCyXDL0_K0CMfV4ghIaiUg1g</t>
-  </si>
-  <si>
     <t>Sporting Kansas City</t>
   </si>
   <si>
@@ -575,6 +572,9 @@
   </si>
   <si>
     <t>https://www.twitter.com/newyorkcityfc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UCVhbRUhe_hfmgi-UN1gcQzw</t>
   </si>
 </sst>
 </file>
@@ -951,14 +951,14 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="F2" sqref="A2:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1606,7 +1606,7 @@
         <v>396242</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H19" t="s">
         <v>113</v>
@@ -1615,7 +1615,7 @@
         <v>114</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K19" t="s">
         <v>115</v>
@@ -1836,7 +1836,7 @@
         <v>152</v>
       </c>
       <c r="B26">
-        <v>399</v>
+        <v>57100</v>
       </c>
       <c r="C26">
         <v>380302</v>
@@ -1863,12 +1863,12 @@
         <v>156</v>
       </c>
       <c r="K26" t="s">
-        <v>157</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B27">
         <v>24900</v>
@@ -1886,24 +1886,24 @@
         <v>395719</v>
       </c>
       <c r="G27" t="s">
+        <v>158</v>
+      </c>
+      <c r="H27" t="s">
         <v>159</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>160</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>161</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>162</v>
-      </c>
-      <c r="K27" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B28">
         <v>12900</v>
@@ -1921,24 +1921,24 @@
         <v>116774</v>
       </c>
       <c r="G28" t="s">
+        <v>164</v>
+      </c>
+      <c r="H28" t="s">
         <v>165</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>166</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>167</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>168</v>
-      </c>
-      <c r="K28" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B29">
         <v>37700</v>
@@ -1956,24 +1956,24 @@
         <v>423718</v>
       </c>
       <c r="G29" t="s">
+        <v>170</v>
+      </c>
+      <c r="H29" t="s">
         <v>171</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>172</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>173</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>174</v>
-      </c>
-      <c r="K29" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B30">
         <v>41200</v>
@@ -1991,19 +1991,19 @@
         <v>330403</v>
       </c>
       <c r="G30" t="s">
+        <v>176</v>
+      </c>
+      <c r="H30" t="s">
         <v>177</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>178</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>179</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>180</v>
-      </c>
-      <c r="K30" t="s">
-        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -2012,5 +2012,6 @@
     <hyperlink ref="J19" r:id="rId2" xr:uid="{AC873013-D56D-49E4-82D7-962322BE027C}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>